<commit_message>
1. Now includes values for ploidy level.
</commit_message>
<xml_diff>
--- a/resources/iscnexamples_test.xlsx
+++ b/resources/iscnexamples_test.xlsx
@@ -1189,8 +1189,8 @@
   </sheetPr>
   <dimension ref="A1:O169"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="B1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100">
-      <selection activeCell="D111" activeCellId="0" pane="topLeft" sqref="D111"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="B3" view="normal" windowProtection="false" workbookViewId="0" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100">
+      <selection activeCell="H3" activeCellId="0" pane="topLeft" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.1"/>
@@ -1257,7 +1257,7 @@
         <v>14</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.5" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
         <v>15</v>
       </c>
@@ -1271,16 +1271,16 @@
         <v>-1</v>
       </c>
       <c r="E2" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F2" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H2" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I2" s="4" t="n">
         <v>0</v>
@@ -1318,16 +1318,16 @@
         <v>-1</v>
       </c>
       <c r="E3" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F3" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H3" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I3" s="4" t="n">
         <v>0</v>
@@ -1365,16 +1365,16 @@
         <v>-1</v>
       </c>
       <c r="E4" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F4" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H4" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I4" s="4" t="n">
         <v>0</v>
@@ -1412,16 +1412,16 @@
         <v>-1</v>
       </c>
       <c r="E5" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F5" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H5" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I5" s="4" t="n">
         <v>0</v>
@@ -1459,16 +1459,16 @@
         <v>1</v>
       </c>
       <c r="E6" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F6" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H6" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I6" s="4" t="n">
         <v>0</v>
@@ -1506,16 +1506,16 @@
         <v>1</v>
       </c>
       <c r="E7" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F7" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G7" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H7" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I7" s="4" t="n">
         <v>0</v>
@@ -1553,16 +1553,16 @@
         <v>1</v>
       </c>
       <c r="E8" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F8" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H8" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I8" s="4" t="n">
         <v>0</v>
@@ -1600,16 +1600,16 @@
         <v>1</v>
       </c>
       <c r="E9" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F9" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H9" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I9" s="4" t="n">
         <v>0</v>
@@ -1647,16 +1647,16 @@
         <v>1</v>
       </c>
       <c r="E10" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F10" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H10" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I10" s="4" t="n">
         <v>0</v>
@@ -1694,16 +1694,16 @@
         <v>-1</v>
       </c>
       <c r="E11" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F11" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H11" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I11" s="4" t="n">
         <v>0</v>
@@ -1741,16 +1741,16 @@
         <v>1</v>
       </c>
       <c r="E12" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F12" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H12" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I12" s="4" t="n">
         <v>0</v>
@@ -1788,16 +1788,16 @@
         <v>1</v>
       </c>
       <c r="E13" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F13" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H13" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I13" s="4" t="n">
         <v>0</v>
@@ -1835,16 +1835,16 @@
         <v>1</v>
       </c>
       <c r="E14" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F14" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H14" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I14" s="4" t="n">
         <v>0</v>
@@ -1882,16 +1882,16 @@
         <v>-1</v>
       </c>
       <c r="E15" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F15" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H15" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I15" s="4" t="n">
         <v>0</v>
@@ -1929,16 +1929,16 @@
         <v>1</v>
       </c>
       <c r="E16" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F16" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H16" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I16" s="4" t="n">
         <v>0</v>
@@ -1976,16 +1976,16 @@
         <v>1</v>
       </c>
       <c r="E17" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F17" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H17" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I17" s="4" t="n">
         <v>0</v>
@@ -2023,16 +2023,16 @@
         <v>1</v>
       </c>
       <c r="E18" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F18" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H18" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I18" s="4" t="n">
         <v>0</v>
@@ -2070,16 +2070,16 @@
         <v>1</v>
       </c>
       <c r="E19" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F19" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H19" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I19" s="4" t="n">
         <v>0</v>
@@ -2117,16 +2117,16 @@
         <v>-1</v>
       </c>
       <c r="E20" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F20" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H20" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I20" s="4" t="n">
         <v>0</v>
@@ -2164,16 +2164,16 @@
         <v>1</v>
       </c>
       <c r="E21" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F21" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H21" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I21" s="4" t="n">
         <v>0</v>
@@ -2211,16 +2211,16 @@
         <v>1</v>
       </c>
       <c r="E22" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F22" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H22" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I22" s="4" t="n">
         <v>0</v>
@@ -2258,16 +2258,16 @@
         <v>1</v>
       </c>
       <c r="E23" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F23" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H23" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I23" s="4" t="n">
         <v>0</v>
@@ -2305,16 +2305,16 @@
         <v>1</v>
       </c>
       <c r="E24" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F24" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H24" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I24" s="4" t="n">
         <v>0</v>
@@ -2352,16 +2352,16 @@
         <v>1</v>
       </c>
       <c r="E25" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F25" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H25" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I25" s="4" t="n">
         <v>0</v>
@@ -2399,16 +2399,16 @@
         <v>-1</v>
       </c>
       <c r="E26" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G26" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H26" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I26" s="4" t="n">
         <v>0</v>
@@ -2446,16 +2446,16 @@
         <v>-1</v>
       </c>
       <c r="E27" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F27" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H27" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I27" s="4" t="n">
         <v>0</v>
@@ -2493,16 +2493,16 @@
         <v>-1</v>
       </c>
       <c r="E28" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F28" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H28" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I28" s="4" t="n">
         <v>0</v>
@@ -2540,16 +2540,16 @@
         <v>-1</v>
       </c>
       <c r="E29" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F29" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H29" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I29" s="4" t="n">
         <v>0</v>
@@ -2587,16 +2587,16 @@
         <v>-1</v>
       </c>
       <c r="E30" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F30" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H30" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I30" s="4" t="n">
         <v>0</v>
@@ -2634,16 +2634,16 @@
         <v>-1</v>
       </c>
       <c r="E31" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F31" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H31" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I31" s="4" t="n">
         <v>0</v>
@@ -2681,16 +2681,16 @@
         <v>1</v>
       </c>
       <c r="E32" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F32" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G32" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H32" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I32" s="4" t="n">
         <v>0</v>
@@ -2728,16 +2728,16 @@
         <v>1</v>
       </c>
       <c r="E33" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F33" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H33" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I33" s="4" t="n">
         <v>0</v>
@@ -2775,16 +2775,16 @@
         <v>1</v>
       </c>
       <c r="E34" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F34" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H34" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I34" s="4" t="n">
         <v>0</v>
@@ -2822,16 +2822,16 @@
         <v>1</v>
       </c>
       <c r="E35" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F35" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G35" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H35" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I35" s="4" t="n">
         <v>0</v>
@@ -2869,16 +2869,16 @@
         <v>1</v>
       </c>
       <c r="E36" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F36" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G36" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H36" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I36" s="4" t="n">
         <v>0</v>
@@ -2916,16 +2916,16 @@
         <v>-1</v>
       </c>
       <c r="E37" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F37" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H37" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I37" s="4" t="n">
         <v>0</v>
@@ -2963,16 +2963,16 @@
         <v>-1</v>
       </c>
       <c r="E38" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F38" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G38" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H38" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I38" s="4" t="n">
         <v>0</v>
@@ -3010,16 +3010,16 @@
         <v>-1</v>
       </c>
       <c r="E39" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F39" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G39" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H39" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I39" s="4" t="n">
         <v>0</v>
@@ -3057,16 +3057,16 @@
         <v>-1</v>
       </c>
       <c r="E40" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F40" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H40" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I40" s="4" t="n">
         <v>0</v>
@@ -3104,16 +3104,16 @@
         <v>-1</v>
       </c>
       <c r="E41" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F41" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G41" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H41" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I41" s="4" t="n">
         <v>0</v>
@@ -3151,16 +3151,16 @@
         <v>-1</v>
       </c>
       <c r="E42" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F42" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G42" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H42" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I42" s="4" t="n">
         <v>0</v>
@@ -3198,16 +3198,16 @@
         <v>-1</v>
       </c>
       <c r="E43" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F43" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G43" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H43" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I43" s="4" t="n">
         <v>0</v>
@@ -3245,16 +3245,16 @@
         <v>-1</v>
       </c>
       <c r="E44" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F44" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G44" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H44" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I44" s="4" t="n">
         <v>0</v>
@@ -3292,16 +3292,16 @@
         <v>-1</v>
       </c>
       <c r="E45" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F45" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G45" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H45" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I45" s="4" t="n">
         <v>0</v>
@@ -3339,16 +3339,16 @@
         <v>-1</v>
       </c>
       <c r="E46" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F46" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G46" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H46" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I46" s="4" t="n">
         <v>0</v>
@@ -3386,16 +3386,16 @@
         <v>-1</v>
       </c>
       <c r="E47" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F47" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G47" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H47" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I47" s="4" t="n">
         <v>0</v>
@@ -3433,16 +3433,16 @@
         <v>-1</v>
       </c>
       <c r="E48" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F48" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G48" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H48" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I48" s="4" t="n">
         <v>0</v>
@@ -3480,16 +3480,16 @@
         <v>-1</v>
       </c>
       <c r="E49" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F49" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G49" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H49" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I49" s="4" t="n">
         <v>0</v>
@@ -3527,16 +3527,16 @@
         <v>-1</v>
       </c>
       <c r="E50" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F50" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G50" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H50" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I50" s="4" t="n">
         <v>0</v>
@@ -3574,16 +3574,16 @@
         <v>-1</v>
       </c>
       <c r="E51" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F51" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G51" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H51" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I51" s="4" t="n">
         <v>0</v>
@@ -3621,16 +3621,16 @@
         <v>-1</v>
       </c>
       <c r="E52" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F52" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G52" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H52" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I52" s="4" t="n">
         <v>0</v>
@@ -3668,16 +3668,16 @@
         <v>-1</v>
       </c>
       <c r="E53" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F53" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G53" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H53" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I53" s="4" t="n">
         <v>0</v>
@@ -3715,16 +3715,16 @@
         <v>-1</v>
       </c>
       <c r="E54" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F54" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G54" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H54" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I54" s="4" t="n">
         <v>0</v>
@@ -3762,16 +3762,16 @@
         <v>-1</v>
       </c>
       <c r="E55" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F55" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G55" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H55" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I55" s="4" t="n">
         <v>0</v>
@@ -3809,16 +3809,16 @@
         <v>-1</v>
       </c>
       <c r="E56" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F56" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G56" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H56" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I56" s="4" t="n">
         <v>0</v>
@@ -3856,16 +3856,16 @@
         <v>-1</v>
       </c>
       <c r="E57" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F57" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G57" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H57" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I57" s="4" t="n">
         <v>0</v>
@@ -3903,16 +3903,16 @@
         <v>-1</v>
       </c>
       <c r="E58" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F58" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G58" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H58" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I58" s="4" t="n">
         <v>0</v>
@@ -3950,16 +3950,16 @@
         <v>-1</v>
       </c>
       <c r="E59" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F59" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G59" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H59" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I59" s="4" t="n">
         <v>0</v>
@@ -3997,16 +3997,16 @@
         <v>-1</v>
       </c>
       <c r="E60" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F60" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G60" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H60" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I60" s="4" t="n">
         <v>0</v>
@@ -4044,16 +4044,16 @@
         <v>-1</v>
       </c>
       <c r="E61" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F61" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G61" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H61" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I61" s="4" t="n">
         <v>0</v>
@@ -4091,16 +4091,16 @@
         <v>-1</v>
       </c>
       <c r="E62" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F62" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G62" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H62" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I62" s="4" t="n">
         <v>0</v>
@@ -4138,16 +4138,16 @@
         <v>-1</v>
       </c>
       <c r="E63" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F63" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G63" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H63" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I63" s="4" t="n">
         <v>0</v>
@@ -4185,16 +4185,16 @@
         <v>-1</v>
       </c>
       <c r="E64" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F64" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G64" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H64" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I64" s="4" t="n">
         <v>0</v>
@@ -4232,16 +4232,16 @@
         <v>-1</v>
       </c>
       <c r="E65" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F65" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G65" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H65" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I65" s="4" t="n">
         <v>0</v>
@@ -4279,16 +4279,16 @@
         <v>-1</v>
       </c>
       <c r="E66" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F66" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G66" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H66" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I66" s="4" t="n">
         <v>0</v>
@@ -4326,16 +4326,16 @@
         <v>-1</v>
       </c>
       <c r="E67" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F67" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G67" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H67" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I67" s="4" t="n">
         <v>0</v>
@@ -4373,16 +4373,16 @@
         <v>-1</v>
       </c>
       <c r="E68" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F68" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G68" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H68" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I68" s="4" t="n">
         <v>0</v>
@@ -4420,16 +4420,16 @@
         <v>-1</v>
       </c>
       <c r="E69" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F69" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G69" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H69" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I69" s="4" t="n">
         <v>0</v>
@@ -4467,16 +4467,16 @@
         <v>-1</v>
       </c>
       <c r="E70" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F70" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G70" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H70" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I70" s="4" t="n">
         <v>0</v>
@@ -4514,16 +4514,16 @@
         <v>-1</v>
       </c>
       <c r="E71" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F71" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G71" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H71" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I71" s="4" t="n">
         <v>0</v>
@@ -4561,16 +4561,16 @@
         <v>-1</v>
       </c>
       <c r="E72" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F72" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G72" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H72" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I72" s="4" t="n">
         <v>0</v>
@@ -4608,16 +4608,16 @@
         <v>-1</v>
       </c>
       <c r="E73" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F73" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G73" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H73" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I73" s="4" t="n">
         <v>0</v>
@@ -4655,16 +4655,16 @@
         <v>-1</v>
       </c>
       <c r="E74" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F74" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G74" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H74" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I74" s="4" t="n">
         <v>0</v>
@@ -4702,16 +4702,16 @@
         <v>-1</v>
       </c>
       <c r="E75" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F75" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G75" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H75" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I75" s="4" t="n">
         <v>0</v>
@@ -4749,16 +4749,16 @@
         <v>-1</v>
       </c>
       <c r="E76" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F76" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G76" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H76" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I76" s="4" t="n">
         <v>0</v>
@@ -4796,16 +4796,16 @@
         <v>-1</v>
       </c>
       <c r="E77" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F77" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G77" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H77" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I77" s="4" t="n">
         <v>0</v>
@@ -4843,16 +4843,16 @@
         <v>-1</v>
       </c>
       <c r="E78" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F78" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G78" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H78" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I78" s="4" t="n">
         <v>0</v>
@@ -4890,16 +4890,16 @@
         <v>-1</v>
       </c>
       <c r="E79" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F79" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G79" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H79" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I79" s="4" t="n">
         <v>0</v>
@@ -4937,16 +4937,16 @@
         <v>-1</v>
       </c>
       <c r="E80" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F80" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G80" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H80" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I80" s="4" t="n">
         <v>0</v>
@@ -4984,16 +4984,16 @@
         <v>-1</v>
       </c>
       <c r="E81" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F81" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G81" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H81" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I81" s="4" t="n">
         <v>0</v>
@@ -5031,16 +5031,16 @@
         <v>-1</v>
       </c>
       <c r="E82" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F82" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G82" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H82" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I82" s="4" t="n">
         <v>0</v>
@@ -5078,16 +5078,16 @@
         <v>-1</v>
       </c>
       <c r="E83" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F83" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G83" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H83" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I83" s="4" t="n">
         <v>0</v>
@@ -5125,16 +5125,16 @@
         <v>-1</v>
       </c>
       <c r="E84" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F84" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G84" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H84" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I84" s="4" t="n">
         <v>0</v>
@@ -5172,16 +5172,16 @@
         <v>-1</v>
       </c>
       <c r="E85" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F85" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G85" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H85" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I85" s="4" t="n">
         <v>0</v>
@@ -5219,16 +5219,16 @@
         <v>-1</v>
       </c>
       <c r="E86" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F86" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G86" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H86" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I86" s="4" t="n">
         <v>0</v>
@@ -5266,16 +5266,16 @@
         <v>-1</v>
       </c>
       <c r="E87" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F87" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G87" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H87" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I87" s="4" t="n">
         <v>0</v>
@@ -5313,16 +5313,16 @@
         <v>-1</v>
       </c>
       <c r="E88" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F88" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G88" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H88" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I88" s="4" t="n">
         <v>0</v>
@@ -5360,16 +5360,16 @@
         <v>1</v>
       </c>
       <c r="E89" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F89" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G89" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H89" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I89" s="4" t="n">
         <v>0</v>
@@ -5407,16 +5407,16 @@
         <v>1</v>
       </c>
       <c r="E90" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F90" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G90" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H90" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I90" s="4" t="n">
         <v>0</v>
@@ -5454,16 +5454,16 @@
         <v>1</v>
       </c>
       <c r="E91" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F91" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G91" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H91" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I91" s="4" t="n">
         <v>0</v>
@@ -5501,16 +5501,16 @@
         <v>1</v>
       </c>
       <c r="E92" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F92" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G92" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H92" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I92" s="4" t="n">
         <v>0</v>
@@ -5548,16 +5548,16 @@
         <v>1</v>
       </c>
       <c r="E93" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F93" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G93" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H93" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I93" s="4" t="n">
         <v>0</v>
@@ -5595,16 +5595,16 @@
         <v>1</v>
       </c>
       <c r="E94" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F94" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G94" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H94" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I94" s="4" t="n">
         <v>0</v>
@@ -5642,16 +5642,16 @@
         <v>1</v>
       </c>
       <c r="E95" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F95" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G95" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H95" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I95" s="4" t="n">
         <v>0</v>
@@ -5689,16 +5689,16 @@
         <v>1</v>
       </c>
       <c r="E96" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F96" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G96" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H96" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I96" s="4" t="n">
         <v>0</v>
@@ -5736,16 +5736,16 @@
         <v>1</v>
       </c>
       <c r="E97" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F97" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G97" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H97" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I97" s="4" t="n">
         <v>0</v>
@@ -5783,16 +5783,16 @@
         <v>1</v>
       </c>
       <c r="E98" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F98" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G98" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H98" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I98" s="4" t="n">
         <v>0</v>
@@ -5830,16 +5830,16 @@
         <v>1</v>
       </c>
       <c r="E99" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F99" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G99" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H99" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I99" s="4" t="n">
         <v>0</v>
@@ -5877,16 +5877,16 @@
         <v>1</v>
       </c>
       <c r="E100" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F100" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G100" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H100" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I100" s="4" t="n">
         <v>0</v>
@@ -5924,16 +5924,16 @@
         <v>1</v>
       </c>
       <c r="E101" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F101" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G101" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H101" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I101" s="4" t="n">
         <v>0</v>
@@ -5971,16 +5971,16 @@
         <v>1</v>
       </c>
       <c r="E102" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F102" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G102" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H102" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I102" s="4" t="n">
         <v>0</v>
@@ -6018,16 +6018,16 @@
         <v>1</v>
       </c>
       <c r="E103" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F103" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G103" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H103" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I103" s="4" t="n">
         <v>0</v>
@@ -6065,16 +6065,16 @@
         <v>1</v>
       </c>
       <c r="E104" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F104" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G104" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H104" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I104" s="4" t="n">
         <v>0</v>
@@ -6112,16 +6112,16 @@
         <v>1</v>
       </c>
       <c r="E105" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F105" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G105" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H105" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I105" s="4" t="n">
         <v>0</v>
@@ -6159,16 +6159,16 @@
         <v>1</v>
       </c>
       <c r="E106" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F106" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G106" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H106" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I106" s="4" t="n">
         <v>0</v>
@@ -6206,16 +6206,16 @@
         <v>1</v>
       </c>
       <c r="E107" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F107" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G107" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H107" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I107" s="4" t="n">
         <v>0</v>
@@ -6253,16 +6253,16 @@
         <v>1</v>
       </c>
       <c r="E108" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F108" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G108" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H108" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I108" s="4" t="n">
         <v>0</v>
@@ -6300,16 +6300,16 @@
         <v>1</v>
       </c>
       <c r="E109" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F109" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G109" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H109" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I109" s="4" t="n">
         <v>0</v>
@@ -6347,16 +6347,16 @@
         <v>1</v>
       </c>
       <c r="E110" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F110" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G110" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H110" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I110" s="4" t="n">
         <v>0</v>
@@ -6394,16 +6394,16 @@
         <v>1</v>
       </c>
       <c r="E111" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F111" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G111" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H111" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I111" s="4" t="n">
         <v>0</v>
@@ -6441,16 +6441,16 @@
         <v>1</v>
       </c>
       <c r="E112" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F112" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G112" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H112" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I112" s="4" t="n">
         <v>0</v>
@@ -6488,16 +6488,16 @@
         <v>-1</v>
       </c>
       <c r="E113" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F113" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G113" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H113" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I113" s="4" t="n">
         <v>0</v>
@@ -6535,16 +6535,16 @@
         <v>-1</v>
       </c>
       <c r="E114" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F114" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G114" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H114" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I114" s="4" t="n">
         <v>0</v>
@@ -6582,16 +6582,16 @@
         <v>1</v>
       </c>
       <c r="E115" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F115" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G115" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H115" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I115" s="4" t="n">
         <v>0</v>
@@ -6629,16 +6629,16 @@
         <v>-1</v>
       </c>
       <c r="E116" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F116" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G116" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H116" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I116" s="4" t="n">
         <v>0</v>
@@ -6676,16 +6676,16 @@
         <v>-1</v>
       </c>
       <c r="E117" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F117" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G117" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H117" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I117" s="4" t="n">
         <v>0</v>
@@ -6723,16 +6723,16 @@
         <v>-1</v>
       </c>
       <c r="E118" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F118" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G118" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H118" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I118" s="4" t="n">
         <v>0</v>
@@ -6770,16 +6770,16 @@
         <v>-1</v>
       </c>
       <c r="E119" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F119" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G119" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H119" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I119" s="4" t="n">
         <v>0</v>
@@ -6817,16 +6817,16 @@
         <v>-1</v>
       </c>
       <c r="E120" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F120" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G120" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H120" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I120" s="4" t="n">
         <v>0</v>
@@ -6864,16 +6864,16 @@
         <v>-1</v>
       </c>
       <c r="E121" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F121" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G121" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H121" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I121" s="4" t="n">
         <v>0</v>
@@ -6911,16 +6911,16 @@
         <v>1</v>
       </c>
       <c r="E122" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F122" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G122" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H122" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I122" s="4" t="n">
         <v>0</v>
@@ -6958,16 +6958,16 @@
         <v>1</v>
       </c>
       <c r="E123" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F123" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G123" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H123" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I123" s="4" t="n">
         <v>0</v>
@@ -7005,16 +7005,16 @@
         <v>1</v>
       </c>
       <c r="E124" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F124" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G124" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H124" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I124" s="4" t="n">
         <v>0</v>
@@ -7052,16 +7052,16 @@
         <v>1</v>
       </c>
       <c r="E125" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F125" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G125" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H125" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I125" s="4" t="n">
         <v>0</v>
@@ -7099,16 +7099,16 @@
         <v>-1</v>
       </c>
       <c r="E126" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F126" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G126" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H126" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I126" s="4" t="n">
         <v>0</v>
@@ -7146,16 +7146,16 @@
         <v>-1</v>
       </c>
       <c r="E127" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F127" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G127" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H127" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I127" s="4" t="n">
         <v>0</v>
@@ -7193,16 +7193,16 @@
         <v>-1</v>
       </c>
       <c r="E128" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F128" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G128" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H128" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I128" s="4" t="n">
         <v>0</v>
@@ -7240,16 +7240,16 @@
         <v>-1</v>
       </c>
       <c r="E129" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F129" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G129" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H129" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I129" s="4" t="n">
         <v>0</v>
@@ -7287,16 +7287,16 @@
         <v>-1</v>
       </c>
       <c r="E130" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F130" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G130" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H130" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I130" s="4" t="n">
         <v>0</v>
@@ -7334,16 +7334,16 @@
         <v>-1</v>
       </c>
       <c r="E131" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F131" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G131" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H131" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I131" s="4" t="n">
         <v>0</v>
@@ -7381,16 +7381,16 @@
         <v>-1</v>
       </c>
       <c r="E132" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F132" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G132" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H132" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I132" s="4" t="n">
         <v>0</v>
@@ -7428,16 +7428,16 @@
         <v>-1</v>
       </c>
       <c r="E133" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F133" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G133" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H133" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I133" s="4" t="n">
         <v>0</v>
@@ -7475,16 +7475,16 @@
         <v>-1</v>
       </c>
       <c r="E134" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F134" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G134" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H134" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I134" s="4" t="n">
         <v>0</v>
@@ -7522,16 +7522,16 @@
         <v>-1</v>
       </c>
       <c r="E135" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F135" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G135" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H135" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I135" s="4" t="n">
         <v>0</v>
@@ -7569,16 +7569,16 @@
         <v>-1</v>
       </c>
       <c r="E136" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F136" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G136" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H136" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I136" s="4" t="n">
         <v>0</v>
@@ -7616,16 +7616,16 @@
         <v>-1</v>
       </c>
       <c r="E137" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F137" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G137" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H137" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I137" s="4" t="n">
         <v>0</v>
@@ -7663,16 +7663,16 @@
         <v>1</v>
       </c>
       <c r="E138" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F138" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G138" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H138" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I138" s="4" t="n">
         <v>0</v>
@@ -7710,16 +7710,16 @@
         <v>1</v>
       </c>
       <c r="E139" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F139" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G139" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H139" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I139" s="4" t="n">
         <v>0</v>
@@ -7757,16 +7757,16 @@
         <v>1</v>
       </c>
       <c r="E140" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F140" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G140" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H140" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I140" s="4" t="n">
         <v>0</v>
@@ -7804,16 +7804,16 @@
         <v>1</v>
       </c>
       <c r="E141" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F141" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G141" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H141" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I141" s="4" t="n">
         <v>0</v>
@@ -7851,16 +7851,16 @@
         <v>1</v>
       </c>
       <c r="E142" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F142" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G142" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H142" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I142" s="4" t="n">
         <v>0</v>
@@ -7898,16 +7898,16 @@
         <v>1</v>
       </c>
       <c r="E143" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F143" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G143" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H143" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I143" s="4" t="n">
         <v>0</v>
@@ -7945,16 +7945,16 @@
         <v>1</v>
       </c>
       <c r="E144" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F144" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G144" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H144" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I144" s="4" t="n">
         <v>0</v>
@@ -7992,16 +7992,16 @@
         <v>-1</v>
       </c>
       <c r="E145" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F145" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G145" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H145" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I145" s="4" t="n">
         <v>0</v>
@@ -8039,16 +8039,16 @@
         <v>1</v>
       </c>
       <c r="E146" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F146" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G146" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H146" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I146" s="4" t="n">
         <v>0</v>
@@ -8086,16 +8086,16 @@
         <v>1</v>
       </c>
       <c r="E147" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F147" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G147" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H147" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I147" s="4" t="n">
         <v>0</v>
@@ -8133,16 +8133,16 @@
         <v>-1</v>
       </c>
       <c r="E148" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F148" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G148" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H148" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I148" s="4" t="n">
         <v>0</v>
@@ -8180,16 +8180,16 @@
         <v>-1</v>
       </c>
       <c r="E149" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F149" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G149" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H149" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I149" s="4" t="n">
         <v>0</v>
@@ -8227,16 +8227,16 @@
         <v>-1</v>
       </c>
       <c r="E150" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F150" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G150" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H150" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I150" s="4" t="n">
         <v>0</v>
@@ -8274,16 +8274,16 @@
         <v>-1</v>
       </c>
       <c r="E151" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F151" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G151" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H151" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I151" s="4" t="n">
         <v>0</v>
@@ -8321,16 +8321,16 @@
         <v>1</v>
       </c>
       <c r="E152" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F152" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G152" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H152" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I152" s="4" t="n">
         <v>0</v>
@@ -8368,16 +8368,16 @@
         <v>1</v>
       </c>
       <c r="E153" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F153" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G153" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H153" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I153" s="4" t="n">
         <v>0</v>
@@ -8415,16 +8415,16 @@
         <v>-1</v>
       </c>
       <c r="E154" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F154" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G154" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H154" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I154" s="4" t="n">
         <v>0</v>
@@ -8462,16 +8462,16 @@
         <v>-1</v>
       </c>
       <c r="E155" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F155" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G155" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H155" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I155" s="4" t="n">
         <v>0</v>
@@ -8509,16 +8509,16 @@
         <v>-1</v>
       </c>
       <c r="E156" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F156" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G156" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H156" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I156" s="4" t="n">
         <v>0</v>
@@ -8556,16 +8556,16 @@
         <v>-1</v>
       </c>
       <c r="E157" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F157" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G157" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H157" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I157" s="4" t="n">
         <v>0</v>
@@ -8603,16 +8603,16 @@
         <v>-1</v>
       </c>
       <c r="E158" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F158" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G158" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H158" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I158" s="4" t="n">
         <v>0</v>
@@ -8650,16 +8650,16 @@
         <v>-1</v>
       </c>
       <c r="E159" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F159" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G159" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H159" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I159" s="4" t="n">
         <v>0</v>
@@ -8697,16 +8697,16 @@
         <v>-1</v>
       </c>
       <c r="E160" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F160" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G160" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H160" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I160" s="4" t="n">
         <v>0</v>
@@ -8744,16 +8744,16 @@
         <v>-1</v>
       </c>
       <c r="E161" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F161" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G161" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H161" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I161" s="4" t="n">
         <v>0</v>
@@ -8791,16 +8791,16 @@
         <v>-1</v>
       </c>
       <c r="E162" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F162" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G162" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H162" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="I162" s="4" t="n">
         <v>0</v>
@@ -8838,16 +8838,16 @@
         <v>-1</v>
       </c>
       <c r="E163" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F163" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G163" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H163" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I163" s="4" t="n">
         <v>0</v>
@@ -8885,16 +8885,16 @@
         <v>-1</v>
       </c>
       <c r="E164" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F164" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G164" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H164" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I164" s="4" t="n">
         <v>0</v>
@@ -8932,16 +8932,16 @@
         <v>-1</v>
       </c>
       <c r="E165" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F165" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G165" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H165" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I165" s="4" t="n">
         <v>0</v>
@@ -8979,16 +8979,16 @@
         <v>-1</v>
       </c>
       <c r="E166" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F166" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G166" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H166" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I166" s="4" t="n">
         <v>0</v>
@@ -9026,16 +9026,16 @@
         <v>-1</v>
       </c>
       <c r="E167" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F167" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G167" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H167" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I167" s="4" t="n">
         <v>0</v>
@@ -9073,16 +9073,16 @@
         <v>-1</v>
       </c>
       <c r="E168" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F168" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G168" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H168" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I168" s="4" t="n">
         <v>0</v>
@@ -9120,16 +9120,16 @@
         <v>-1</v>
       </c>
       <c r="E169" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F169" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G169" s="4" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="H169" s="4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I169" s="4" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
1. Included instances for Deletion, Duplication, Fission, Insertion, Inversion, Quadruplication, Translocation and Triplication events.
</commit_message>
<xml_diff>
--- a/resources/iscnexamples_test.xlsx
+++ b/resources/iscnexamples_test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="356">
   <si>
     <t>Name</t>
   </si>
@@ -1064,6 +1064,24 @@
   </si>
   <si>
     <t>Addition</t>
+  </si>
+  <si>
+    <t>Deletion</t>
+  </si>
+  <si>
+    <t>Duplication</t>
+  </si>
+  <si>
+    <t>Fission</t>
+  </si>
+  <si>
+    <t>Insertion</t>
+  </si>
+  <si>
+    <t>Translocation</t>
+  </si>
+  <si>
+    <t>Triplication</t>
   </si>
 </sst>
 </file>
@@ -1423,23 +1441,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N169"/>
+  <dimension ref="A1:T169"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="O91" sqref="O91"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="54.28515625"/>
-    <col min="2" max="12" width="0" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875"/>
-    <col min="16" max="1025" width="11.5703125"/>
+    <col min="1" max="2" width="46.5703125" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.7109375" customWidth="1"/>
+    <col min="15" max="15" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1482,8 +1514,26 @@
       <c r="N1" s="5" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O1" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1526,8 +1576,26 @@
       <c r="N2" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O2" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P2" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R2" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S2" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T2" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1570,8 +1638,26 @@
       <c r="N3" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T3" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1614,8 +1700,26 @@
       <c r="N4" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T4" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1658,8 +1762,26 @@
       <c r="N5" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O5" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P5" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R5" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S5" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T5" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1702,8 +1824,26 @@
       <c r="N6" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O6" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P6" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R6" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S6" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T6" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1746,8 +1886,26 @@
       <c r="N7" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O7" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P7" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R7" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S7" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T7" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1790,8 +1948,26 @@
       <c r="N8" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O8" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P8" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R8" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S8" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T8" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1834,8 +2010,26 @@
       <c r="N9" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O9" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P9" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R9" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S9" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T9" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1878,8 +2072,26 @@
       <c r="N10" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O10" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P10" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R10" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S10" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T10" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1922,8 +2134,26 @@
       <c r="N11" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O11" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P11" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R11" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S11" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T11" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1966,8 +2196,26 @@
       <c r="N12" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O12" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P12" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R12" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S12" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T12" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -2010,8 +2258,26 @@
       <c r="N13" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O13" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P13" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R13" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S13" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T13" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -2054,8 +2320,26 @@
       <c r="N14" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O14" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P14" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R14" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S14" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T14" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -2098,8 +2382,26 @@
       <c r="N15" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O15" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P15" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R15" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S15" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T15" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -2142,8 +2444,26 @@
       <c r="N16" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O16" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P16" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R16" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S16" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T16" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -2186,8 +2506,26 @@
       <c r="N17" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O17" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P17" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R17" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S17" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T17" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -2230,8 +2568,26 @@
       <c r="N18" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O18" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P18" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R18" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S18" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T18" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -2274,8 +2630,26 @@
       <c r="N19" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O19" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P19" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R19" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S19" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T19" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -2318,8 +2692,26 @@
       <c r="N20" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O20" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P20" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R20" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S20" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T20" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -2362,8 +2754,26 @@
       <c r="N21" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O21" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P21" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R21" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S21" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T21" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -2406,8 +2816,26 @@
       <c r="N22" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O22" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P22" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R22" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S22" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T22" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -2450,8 +2878,26 @@
       <c r="N23" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O23" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P23" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q23" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R23" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S23" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T23" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -2494,8 +2940,26 @@
       <c r="N24" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O24" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P24" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R24" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S24" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T24" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -2538,8 +3002,26 @@
       <c r="N25" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O25" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P25" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R25" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S25" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T25" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>61</v>
       </c>
@@ -2582,8 +3064,26 @@
       <c r="N26" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O26" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P26" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R26" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S26" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T26" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>63</v>
       </c>
@@ -2626,8 +3126,26 @@
       <c r="N27" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O27" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P27" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q27" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R27" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S27" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T27" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>65</v>
       </c>
@@ -2670,8 +3188,26 @@
       <c r="N28" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O28" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P28" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R28" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S28" s="1">
+        <v>1</v>
+      </c>
+      <c r="T28" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>67</v>
       </c>
@@ -2714,8 +3250,26 @@
       <c r="N29" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O29" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P29" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R29" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S29" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T29" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>69</v>
       </c>
@@ -2758,8 +3312,26 @@
       <c r="N30" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O30" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P30" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q30" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R30" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S30" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T30" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>71</v>
       </c>
@@ -2802,8 +3374,26 @@
       <c r="N31" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O31" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P31" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q31" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R31" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S31" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T31" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>73</v>
       </c>
@@ -2846,8 +3436,26 @@
       <c r="N32" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O32" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P32" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R32" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S32" s="1">
+        <v>1</v>
+      </c>
+      <c r="T32" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>75</v>
       </c>
@@ -2890,8 +3498,26 @@
       <c r="N33" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O33" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P33" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q33" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R33" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S33" s="1">
+        <v>1</v>
+      </c>
+      <c r="T33" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>77</v>
       </c>
@@ -2934,8 +3560,26 @@
       <c r="N34" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O34" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P34" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q34" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R34" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S34" s="1">
+        <v>1</v>
+      </c>
+      <c r="T34" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>79</v>
       </c>
@@ -2978,8 +3622,26 @@
       <c r="N35" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O35" s="1">
+        <v>1</v>
+      </c>
+      <c r="P35" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q35" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R35" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S35" s="1">
+        <v>1</v>
+      </c>
+      <c r="T35" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>81</v>
       </c>
@@ -3022,8 +3684,26 @@
       <c r="N36" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O36" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P36" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q36" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R36" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S36" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T36" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>83</v>
       </c>
@@ -3066,8 +3746,26 @@
       <c r="N37" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O37" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P37" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q37" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R37" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S37" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T37" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>85</v>
       </c>
@@ -3110,8 +3808,26 @@
       <c r="N38" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O38" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P38" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q38" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R38" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S38" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T38" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>87</v>
       </c>
@@ -3154,8 +3870,26 @@
       <c r="N39" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O39" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P39" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q39" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R39" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S39" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T39" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>89</v>
       </c>
@@ -3198,8 +3932,26 @@
       <c r="N40" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O40" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P40" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q40" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R40" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S40" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T40" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>91</v>
       </c>
@@ -3242,8 +3994,26 @@
       <c r="N41" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O41" s="1">
+        <v>1</v>
+      </c>
+      <c r="P41" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q41" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R41" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S41" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T41" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>93</v>
       </c>
@@ -3286,8 +4056,26 @@
       <c r="N42" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O42" s="1">
+        <v>1</v>
+      </c>
+      <c r="P42" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q42" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R42" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S42" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T42" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>95</v>
       </c>
@@ -3330,8 +4118,26 @@
       <c r="N43" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O43" s="1">
+        <v>1</v>
+      </c>
+      <c r="P43" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q43" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R43" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S43" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T43" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>97</v>
       </c>
@@ -3374,8 +4180,26 @@
       <c r="N44" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O44" s="1">
+        <v>1</v>
+      </c>
+      <c r="P44" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q44" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R44" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S44" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T44" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>99</v>
       </c>
@@ -3418,8 +4242,26 @@
       <c r="N45" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O45" s="1">
+        <v>1</v>
+      </c>
+      <c r="P45" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q45" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R45" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S45" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T45" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>101</v>
       </c>
@@ -3462,8 +4304,26 @@
       <c r="N46" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O46" s="1">
+        <v>1</v>
+      </c>
+      <c r="P46" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q46" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R46" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S46" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T46" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>103</v>
       </c>
@@ -3506,8 +4366,26 @@
       <c r="N47" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O47" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P47" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q47" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R47" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S47" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T47" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>105</v>
       </c>
@@ -3550,8 +4428,26 @@
       <c r="N48" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O48" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P48" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q48" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R48" s="1">
+        <v>1</v>
+      </c>
+      <c r="S48" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T48" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>107</v>
       </c>
@@ -3594,8 +4490,26 @@
       <c r="N49" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O49" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P49" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q49" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R49" s="1">
+        <v>1</v>
+      </c>
+      <c r="S49" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T49" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>109</v>
       </c>
@@ -3638,8 +4552,26 @@
       <c r="N50" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O50" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P50" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q50" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R50" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S50" s="1">
+        <v>1</v>
+      </c>
+      <c r="T50" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>111</v>
       </c>
@@ -3682,8 +4614,26 @@
       <c r="N51" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O51" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P51" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q51" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R51" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S51" s="1">
+        <v>1</v>
+      </c>
+      <c r="T51" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>113</v>
       </c>
@@ -3726,8 +4676,26 @@
       <c r="N52" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O52" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P52" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q52" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R52" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S52" s="1">
+        <v>1</v>
+      </c>
+      <c r="T52" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>115</v>
       </c>
@@ -3770,8 +4738,26 @@
       <c r="N53" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O53" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P53" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q53" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R53" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S53" s="1">
+        <v>1</v>
+      </c>
+      <c r="T53" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>117</v>
       </c>
@@ -3814,8 +4800,26 @@
       <c r="N54" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O54" s="1">
+        <v>1</v>
+      </c>
+      <c r="P54" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q54" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R54" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S54" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T54" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>119</v>
       </c>
@@ -3858,8 +4862,26 @@
       <c r="N55" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O55" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P55" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q55" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R55" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S55" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T55" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>121</v>
       </c>
@@ -3902,8 +4924,26 @@
       <c r="N56" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O56" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P56" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q56" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R56" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S56" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T56" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>123</v>
       </c>
@@ -3946,8 +4986,26 @@
       <c r="N57" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O57" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P57" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q57" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R57" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S57" s="1">
+        <v>1</v>
+      </c>
+      <c r="T57" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>125</v>
       </c>
@@ -3990,8 +5048,26 @@
       <c r="N58" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O58" s="1">
+        <v>1</v>
+      </c>
+      <c r="P58" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q58" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R58" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S58" s="1">
+        <v>1</v>
+      </c>
+      <c r="T58" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>127</v>
       </c>
@@ -4034,8 +5110,26 @@
       <c r="N59" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O59" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P59" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q59" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R59" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S59" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T59" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>129</v>
       </c>
@@ -4078,8 +5172,26 @@
       <c r="N60" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O60" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P60" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q60" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R60" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S60" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T60" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>131</v>
       </c>
@@ -4122,8 +5234,26 @@
       <c r="N61" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O61" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P61" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q61" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R61" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S61" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T61" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>133</v>
       </c>
@@ -4166,8 +5296,26 @@
       <c r="N62" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O62" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P62" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q62" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R62" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S62" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T62" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>135</v>
       </c>
@@ -4210,8 +5358,26 @@
       <c r="N63" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O63" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P63" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q63" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R63" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S63" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T63" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>137</v>
       </c>
@@ -4254,8 +5420,26 @@
       <c r="N64" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O64" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P64" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q64" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R64" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S64" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T64" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>139</v>
       </c>
@@ -4298,8 +5482,26 @@
       <c r="N65" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O65" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P65" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q65" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R65" s="1">
+        <v>1</v>
+      </c>
+      <c r="S65" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T65" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>141</v>
       </c>
@@ -4342,8 +5544,26 @@
       <c r="N66" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O66" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P66" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q66" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R66" s="1">
+        <v>1</v>
+      </c>
+      <c r="S66" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T66" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>143</v>
       </c>
@@ -4386,8 +5606,26 @@
       <c r="N67" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O67" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P67" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q67" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R67" s="1">
+        <v>1</v>
+      </c>
+      <c r="S67" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T67" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>145</v>
       </c>
@@ -4430,8 +5668,26 @@
       <c r="N68" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O68" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P68" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q68" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R68" s="1">
+        <v>1</v>
+      </c>
+      <c r="S68" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T68" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>147</v>
       </c>
@@ -4474,8 +5730,26 @@
       <c r="N69" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O69" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P69" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q69" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R69" s="1">
+        <v>1</v>
+      </c>
+      <c r="S69" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T69" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>149</v>
       </c>
@@ -4518,8 +5792,26 @@
       <c r="N70" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O70" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P70" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q70" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R70" s="1">
+        <v>1</v>
+      </c>
+      <c r="S70" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T70" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>151</v>
       </c>
@@ -4562,8 +5854,26 @@
       <c r="N71" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O71" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P71" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q71" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R71" s="1">
+        <v>1</v>
+      </c>
+      <c r="S71" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T71" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>153</v>
       </c>
@@ -4606,8 +5916,26 @@
       <c r="N72" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O72" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P72" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q72" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R72" s="1">
+        <v>1</v>
+      </c>
+      <c r="S72" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T72" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>155</v>
       </c>
@@ -4650,8 +5978,26 @@
       <c r="N73" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O73" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P73" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q73" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R73" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S73" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T73" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>157</v>
       </c>
@@ -4694,8 +6040,26 @@
       <c r="N74" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O74" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P74" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q74" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R74" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S74" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T74" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>159</v>
       </c>
@@ -4738,8 +6102,26 @@
       <c r="N75" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O75" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P75" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q75" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R75" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S75" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T75" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>161</v>
       </c>
@@ -4782,8 +6164,26 @@
       <c r="N76" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O76" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P76" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q76" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R76" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S76" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T76" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>163</v>
       </c>
@@ -4826,8 +6226,26 @@
       <c r="N77" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O77" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P77" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q77" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R77" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S77" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T77" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>165</v>
       </c>
@@ -4870,8 +6288,26 @@
       <c r="N78" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O78" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P78" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q78" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R78" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S78" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T78" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>167</v>
       </c>
@@ -4914,8 +6350,26 @@
       <c r="N79" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O79" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P79" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q79" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R79" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S79" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T79" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>169</v>
       </c>
@@ -4958,8 +6412,26 @@
       <c r="N80" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O80" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P80" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q80" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R80" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S80" s="1">
+        <v>1</v>
+      </c>
+      <c r="T80" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>171</v>
       </c>
@@ -5002,8 +6474,26 @@
       <c r="N81" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O81" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P81" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q81" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R81" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S81" s="1">
+        <v>1</v>
+      </c>
+      <c r="T81" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>173</v>
       </c>
@@ -5046,8 +6536,26 @@
       <c r="N82" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O82" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P82" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q82" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R82" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S82" s="1">
+        <v>1</v>
+      </c>
+      <c r="T82" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>175</v>
       </c>
@@ -5090,8 +6598,26 @@
       <c r="N83" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O83" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P83" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q83" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R83" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S83" s="1">
+        <v>1</v>
+      </c>
+      <c r="T83" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>177</v>
       </c>
@@ -5134,8 +6660,26 @@
       <c r="N84" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O84" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P84" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q84" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R84" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S84" s="1">
+        <v>1</v>
+      </c>
+      <c r="T84" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>179</v>
       </c>
@@ -5178,8 +6722,26 @@
       <c r="N85" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O85" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P85" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q85" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R85" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S85" s="1">
+        <v>1</v>
+      </c>
+      <c r="T85" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>181</v>
       </c>
@@ -5222,8 +6784,26 @@
       <c r="N86" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O86" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P86" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q86" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R86" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S86" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T86" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>183</v>
       </c>
@@ -5266,8 +6846,26 @@
       <c r="N87" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O87" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P87" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q87" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R87" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S87" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T87" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>185</v>
       </c>
@@ -5310,8 +6908,26 @@
       <c r="N88" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O88" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P88" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q88" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R88" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S88" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T88" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>187</v>
       </c>
@@ -5354,8 +6970,26 @@
       <c r="N89" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O89" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P89" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q89" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R89" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S89" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T89" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>189</v>
       </c>
@@ -5398,8 +7032,26 @@
       <c r="N90" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O90" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P90" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q90" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R90" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S90" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T90" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>191</v>
       </c>
@@ -5442,8 +7094,26 @@
       <c r="N91" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O91" s="1">
+        <v>1</v>
+      </c>
+      <c r="P91" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q91" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R91" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S91" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T91" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>193</v>
       </c>
@@ -5486,8 +7156,26 @@
       <c r="N92" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O92" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P92" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q92" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R92" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S92" s="1">
+        <v>1</v>
+      </c>
+      <c r="T92" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>195</v>
       </c>
@@ -5530,8 +7218,26 @@
       <c r="N93" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O93" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P93" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q93" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R93" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S93" s="1">
+        <v>1</v>
+      </c>
+      <c r="T93" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>197</v>
       </c>
@@ -5574,8 +7280,26 @@
       <c r="N94" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O94" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P94" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q94" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R94" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S94" s="1">
+        <v>1</v>
+      </c>
+      <c r="T94" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>199</v>
       </c>
@@ -5618,8 +7342,26 @@
       <c r="N95" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O95" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P95" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q95" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R95" s="1">
+        <v>1</v>
+      </c>
+      <c r="S95" s="1">
+        <v>1</v>
+      </c>
+      <c r="T95" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>201</v>
       </c>
@@ -5662,8 +7404,26 @@
       <c r="N96" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O96" s="1">
+        <v>1</v>
+      </c>
+      <c r="P96" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q96" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R96" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S96" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T96" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>203</v>
       </c>
@@ -5706,8 +7466,26 @@
       <c r="N97" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O97" s="1">
+        <v>1</v>
+      </c>
+      <c r="P97" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q97" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R97" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S97" s="1">
+        <v>1</v>
+      </c>
+      <c r="T97" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>205</v>
       </c>
@@ -5750,8 +7528,26 @@
       <c r="N98" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O98" s="1">
+        <v>1</v>
+      </c>
+      <c r="P98" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q98" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R98" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S98" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T98" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>207</v>
       </c>
@@ -5794,8 +7590,26 @@
       <c r="N99" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O99" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P99" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q99" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R99" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S99" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T99" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>209</v>
       </c>
@@ -5838,8 +7652,26 @@
       <c r="N100" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O100" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P100" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q100" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R100" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S100" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T100" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>211</v>
       </c>
@@ -5882,8 +7714,26 @@
       <c r="N101" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O101" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P101" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q101" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R101" s="1">
+        <v>1</v>
+      </c>
+      <c r="S101" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T101" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>213</v>
       </c>
@@ -5926,8 +7776,26 @@
       <c r="N102" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O102" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P102" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q102" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R102" s="1">
+        <v>1</v>
+      </c>
+      <c r="S102" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T102" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>215</v>
       </c>
@@ -5970,8 +7838,26 @@
       <c r="N103" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O103" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P103" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q103" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R103" s="1">
+        <v>1</v>
+      </c>
+      <c r="S103" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T103" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>217</v>
       </c>
@@ -6014,8 +7900,26 @@
       <c r="N104" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O104" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P104" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q104" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R104" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S104" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T104" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>219</v>
       </c>
@@ -6058,8 +7962,26 @@
       <c r="N105" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O105" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P105" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q105" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R105" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S105" s="1">
+        <v>1</v>
+      </c>
+      <c r="T105" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>221</v>
       </c>
@@ -6102,8 +8024,26 @@
       <c r="N106" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O106" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P106" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q106" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R106" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S106" s="1">
+        <v>1</v>
+      </c>
+      <c r="T106" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>223</v>
       </c>
@@ -6146,8 +8086,26 @@
       <c r="N107" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O107" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P107" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q107" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R107" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S107" s="1">
+        <v>1</v>
+      </c>
+      <c r="T107" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>225</v>
       </c>
@@ -6190,8 +8148,26 @@
       <c r="N108" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O108" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P108" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q108" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R108" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S108" s="1">
+        <v>1</v>
+      </c>
+      <c r="T108" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>227</v>
       </c>
@@ -6234,8 +8210,26 @@
       <c r="N109" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O109" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P109" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q109" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R109" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S109" s="1">
+        <v>1</v>
+      </c>
+      <c r="T109" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>229</v>
       </c>
@@ -6278,8 +8272,26 @@
       <c r="N110" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O110" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P110" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q110" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R110" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S110" s="1">
+        <v>1</v>
+      </c>
+      <c r="T110" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>231</v>
       </c>
@@ -6322,8 +8334,26 @@
       <c r="N111" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O111" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P111" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q111" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R111" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S111" s="1">
+        <v>1</v>
+      </c>
+      <c r="T111" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>233</v>
       </c>
@@ -6366,8 +8396,26 @@
       <c r="N112" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O112" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P112" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q112" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R112" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S112" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T112" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>235</v>
       </c>
@@ -6410,8 +8458,26 @@
       <c r="N113" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O113" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P113" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q113" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R113" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S113" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T113" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>237</v>
       </c>
@@ -6454,8 +8520,26 @@
       <c r="N114" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O114" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P114" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q114" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R114" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S114" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T114" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>239</v>
       </c>
@@ -6498,8 +8582,26 @@
       <c r="N115" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O115" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P115" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q115" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R115" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S115" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T115" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>241</v>
       </c>
@@ -6542,8 +8644,26 @@
       <c r="N116" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O116" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P116" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q116" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R116" s="1">
+        <v>1</v>
+      </c>
+      <c r="S116" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T116" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>243</v>
       </c>
@@ -6586,8 +8706,26 @@
       <c r="N117" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O117" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P117" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q117" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R117" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S117" s="1">
+        <v>1</v>
+      </c>
+      <c r="T117" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>245</v>
       </c>
@@ -6630,8 +8768,26 @@
       <c r="N118" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O118" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P118" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q118" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R118" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S118" s="1">
+        <v>1</v>
+      </c>
+      <c r="T118" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>247</v>
       </c>
@@ -6674,8 +8830,26 @@
       <c r="N119" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O119" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P119" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q119" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R119" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S119" s="1">
+        <v>1</v>
+      </c>
+      <c r="T119" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>249</v>
       </c>
@@ -6718,8 +8892,26 @@
       <c r="N120" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O120" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P120" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q120" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R120" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S120" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T120" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>251</v>
       </c>
@@ -6762,8 +8954,26 @@
       <c r="N121" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O121" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P121" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q121" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R121" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S121" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T121" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>253</v>
       </c>
@@ -6806,8 +9016,26 @@
       <c r="N122" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O122" s="1">
+        <v>1</v>
+      </c>
+      <c r="P122" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q122" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R122" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S122" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T122" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>255</v>
       </c>
@@ -6850,8 +9078,26 @@
       <c r="N123" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O123" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P123" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q123" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R123" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S123" s="1">
+        <v>1</v>
+      </c>
+      <c r="T123" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>257</v>
       </c>
@@ -6894,8 +9140,26 @@
       <c r="N124" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O124" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P124" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q124" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R124" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S124" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T124" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>259</v>
       </c>
@@ -6938,8 +9202,26 @@
       <c r="N125" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O125" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P125" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q125" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R125" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S125" s="1">
+        <v>1</v>
+      </c>
+      <c r="T125" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>261</v>
       </c>
@@ -6982,8 +9264,26 @@
       <c r="N126" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O126" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P126" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q126" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R126" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S126" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T126" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>263</v>
       </c>
@@ -7026,8 +9326,26 @@
       <c r="N127" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O127" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P127" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q127" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R127" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S127" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T127" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>265</v>
       </c>
@@ -7070,8 +9388,26 @@
       <c r="N128" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O128" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P128" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q128" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R128" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S128" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T128" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>267</v>
       </c>
@@ -7114,8 +9450,26 @@
       <c r="N129" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O129" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P129" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q129" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R129" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S129" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T129" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>269</v>
       </c>
@@ -7158,8 +9512,26 @@
       <c r="N130" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O130" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P130" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q130" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R130" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S130" s="1">
+        <v>1</v>
+      </c>
+      <c r="T130" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>271</v>
       </c>
@@ -7202,8 +9574,26 @@
       <c r="N131" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O131" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P131" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q131" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R131" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S131" s="1">
+        <v>1</v>
+      </c>
+      <c r="T131" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>273</v>
       </c>
@@ -7246,8 +9636,26 @@
       <c r="N132" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O132" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P132" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q132" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R132" s="1">
+        <v>1</v>
+      </c>
+      <c r="S132" s="1">
+        <v>1</v>
+      </c>
+      <c r="T132" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>275</v>
       </c>
@@ -7290,8 +9698,26 @@
       <c r="N133" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O133" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P133" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q133" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R133" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S133" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T133" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>277</v>
       </c>
@@ -7334,8 +9760,26 @@
       <c r="N134" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O134" s="1">
+        <v>1</v>
+      </c>
+      <c r="P134" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q134" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R134" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S134" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T134" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>279</v>
       </c>
@@ -7378,8 +9822,26 @@
       <c r="N135" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O135" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P135" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q135" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R135" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S135" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T135" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>281</v>
       </c>
@@ -7422,8 +9884,26 @@
       <c r="N136" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O136" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P136" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q136" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R136" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S136" s="1">
+        <v>1</v>
+      </c>
+      <c r="T136" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>283</v>
       </c>
@@ -7466,8 +9946,26 @@
       <c r="N137" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O137" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P137" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q137" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R137" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S137" s="1">
+        <v>1</v>
+      </c>
+      <c r="T137" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>285</v>
       </c>
@@ -7510,8 +10008,26 @@
       <c r="N138" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O138" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P138" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q138" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R138" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S138" s="1">
+        <v>1</v>
+      </c>
+      <c r="T138" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>287</v>
       </c>
@@ -7554,8 +10070,26 @@
       <c r="N139" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O139" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P139" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q139" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R139" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S139" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T139" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>289</v>
       </c>
@@ -7598,8 +10132,26 @@
       <c r="N140" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O140" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P140" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q140" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R140" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S140" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T140" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>291</v>
       </c>
@@ -7642,8 +10194,26 @@
       <c r="N141" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O141" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P141" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q141" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R141" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S141" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T141" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>293</v>
       </c>
@@ -7686,8 +10256,26 @@
       <c r="N142" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O142" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P142" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q142" s="1">
+        <v>1</v>
+      </c>
+      <c r="R142" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S142" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T142" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>295</v>
       </c>
@@ -7730,8 +10318,26 @@
       <c r="N143" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O143" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P143" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q143" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R143" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S143" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T143" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>297</v>
       </c>
@@ -7774,8 +10380,26 @@
       <c r="N144" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O144" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P144" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q144" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R144" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S144" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T144" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>299</v>
       </c>
@@ -7818,8 +10442,26 @@
       <c r="N145" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O145" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P145" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q145" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R145" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S145" s="1">
+        <v>1</v>
+      </c>
+      <c r="T145" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>301</v>
       </c>
@@ -7862,8 +10504,26 @@
       <c r="N146" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O146" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P146" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q146" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R146" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S146" s="1">
+        <v>1</v>
+      </c>
+      <c r="T146" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>303</v>
       </c>
@@ -7906,8 +10566,26 @@
       <c r="N147" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O147" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P147" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q147" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R147" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S147" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T147" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>305</v>
       </c>
@@ -7950,8 +10628,26 @@
       <c r="N148" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O148" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P148" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q148" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R148" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S148" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T148" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>307</v>
       </c>
@@ -7994,8 +10690,26 @@
       <c r="N149" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O149" s="1">
+        <v>1</v>
+      </c>
+      <c r="P149" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q149" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R149" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S149" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T149" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>309</v>
       </c>
@@ -8038,8 +10752,26 @@
       <c r="N150" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O150" s="1">
+        <v>1</v>
+      </c>
+      <c r="P150" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q150" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R150" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S150" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T150" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>311</v>
       </c>
@@ -8082,8 +10814,26 @@
       <c r="N151" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O151" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P151" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q151" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R151" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S151" s="1">
+        <v>1</v>
+      </c>
+      <c r="T151" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>313</v>
       </c>
@@ -8126,8 +10876,26 @@
       <c r="N152" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O152" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P152" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q152" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R152" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S152" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T152" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>315</v>
       </c>
@@ -8170,8 +10938,26 @@
       <c r="N153" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O153" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P153" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q153" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R153" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S153" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T153" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>317</v>
       </c>
@@ -8214,8 +11000,26 @@
       <c r="N154" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O154" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P154" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q154" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R154" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S154" s="1">
+        <v>1</v>
+      </c>
+      <c r="T154" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>319</v>
       </c>
@@ -8258,8 +11062,26 @@
       <c r="N155" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O155" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P155" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q155" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R155" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S155" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T155" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>321</v>
       </c>
@@ -8302,8 +11124,26 @@
       <c r="N156" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O156" s="1">
+        <v>1</v>
+      </c>
+      <c r="P156" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q156" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R156" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S156" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T156" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>323</v>
       </c>
@@ -8346,8 +11186,26 @@
       <c r="N157" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O157" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P157" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q157" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R157" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S157" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T157" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>325</v>
       </c>
@@ -8390,8 +11248,26 @@
       <c r="N158" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O158" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P158" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q158" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R158" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S158" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T158" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>327</v>
       </c>
@@ -8434,8 +11310,26 @@
       <c r="N159" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O159" s="1">
+        <v>1</v>
+      </c>
+      <c r="P159" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q159" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R159" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S159" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T159" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>329</v>
       </c>
@@ -8478,8 +11372,26 @@
       <c r="N160" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O160" s="1">
+        <v>1</v>
+      </c>
+      <c r="P160" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q160" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R160" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S160" s="1">
+        <v>1</v>
+      </c>
+      <c r="T160" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>331</v>
       </c>
@@ -8522,8 +11434,26 @@
       <c r="N161" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O161" s="1">
+        <v>1</v>
+      </c>
+      <c r="P161" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q161" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R161" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S161" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T161" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>333</v>
       </c>
@@ -8566,8 +11496,26 @@
       <c r="N162" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O162" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P162" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q162" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R162" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S162" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T162" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>335</v>
       </c>
@@ -8610,8 +11558,26 @@
       <c r="N163" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O163" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P163" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q163" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R163" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S163" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T163" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>337</v>
       </c>
@@ -8654,8 +11620,26 @@
       <c r="N164" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O164" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P164" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q164" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R164" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S164" s="1">
+        <v>1</v>
+      </c>
+      <c r="T164" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>339</v>
       </c>
@@ -8698,8 +11682,26 @@
       <c r="N165" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O165" s="1">
+        <v>1</v>
+      </c>
+      <c r="P165" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q165" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R165" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S165" s="1">
+        <v>-1</v>
+      </c>
+      <c r="T165" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>341</v>
       </c>
@@ -8742,8 +11744,26 @@
       <c r="N166" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O166" s="1">
+        <v>1</v>
+      </c>
+      <c r="P166" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q166" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R166" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S166" s="1">
+        <v>1</v>
+      </c>
+      <c r="T166" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>343</v>
       </c>
@@ -8786,8 +11806,26 @@
       <c r="N167" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="168" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O167" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P167" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q167" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R167" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S167" s="1">
+        <v>1</v>
+      </c>
+      <c r="T167" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>345</v>
       </c>
@@ -8830,8 +11868,26 @@
       <c r="N168" s="1">
         <v>-1</v>
       </c>
-    </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O168" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P168" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q168" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R168" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S168" s="1">
+        <v>1</v>
+      </c>
+      <c r="T168" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>347</v>
       </c>
@@ -8872,6 +11928,24 @@
         <v>-1</v>
       </c>
       <c r="N169" s="1">
+        <v>-1</v>
+      </c>
+      <c r="O169" s="1">
+        <v>-1</v>
+      </c>
+      <c r="P169" s="1">
+        <v>-1</v>
+      </c>
+      <c r="Q169" s="1">
+        <v>-1</v>
+      </c>
+      <c r="R169" s="1">
+        <v>-1</v>
+      </c>
+      <c r="S169" s="1">
+        <v>1</v>
+      </c>
+      <c r="T169" s="1">
         <v>-1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1. Included definitiion (and test) for mosiac karyotype.
</commit_message>
<xml_diff>
--- a/resources/iscnexamples_test.xlsx
+++ b/resources/iscnexamples_test.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="357">
   <si>
     <t>Name</t>
   </si>
@@ -1083,6 +1083,9 @@
   </si>
   <si>
     <t>94,XXYY,t(8,14)(q24.1,q32)x2,+der(14)t(8,14)x2</t>
+  </si>
+  <si>
+    <t>kmos_47_XXY!10!_46_XY!20!</t>
   </si>
 </sst>
 </file>
@@ -1164,7 +1167,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -1185,6 +1188,10 @@
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -1202,16 +1209,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T169"/>
+  <dimension ref="A1:T170"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="P121" view="normal" windowProtection="false" workbookViewId="0" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100">
-      <selection activeCell="S137" activeCellId="0" pane="topLeft" sqref="S137"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="L160" view="normal" windowProtection="false" workbookViewId="0" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100">
+      <selection activeCell="T170" activeCellId="0" pane="topLeft" sqref="T170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.5714285714286"/>
-    <col collapsed="false" hidden="true" max="13" min="2" style="0" width="0"/>
+    <col collapsed="false" hidden="false" max="13" min="2" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.71428571428571"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.85714285714286"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="10.2857142857143"/>
@@ -9654,7 +9661,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.75" outlineLevel="0" r="137">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="137">
       <c r="A137" s="0" t="s">
         <v>290</v>
       </c>
@@ -11698,6 +11705,66 @@
       </c>
       <c r="T169" s="3" t="n">
         <v>-1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.5" outlineLevel="0" r="170">
+      <c r="A170" s="0" t="s">
+        <v>356</v>
+      </c>
+      <c r="B170" s="5"/>
+      <c r="C170" s="5" t="n">
+        <v>-1</v>
+      </c>
+      <c r="D170" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E170" s="5" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F170" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G170" s="5" t="n">
+        <v>-1</v>
+      </c>
+      <c r="H170" s="5" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I170" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J170" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K170" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L170" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M170" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N170" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O170" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P170" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q170" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R170" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S170" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T170" s="5" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated parse column -- again
</commit_message>
<xml_diff>
--- a/resources/iscnexamples_test.xlsx
+++ b/resources/iscnexamples_test.xlsx
@@ -1452,8 +1452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="C102" sqref="C102"/>
+    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
+      <selection activeCell="C125" sqref="C125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8955,7 +8955,7 @@
         <v>249</v>
       </c>
       <c r="C116" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D116" s="3">
         <v>1</v>
@@ -9020,7 +9020,7 @@
         <v>251</v>
       </c>
       <c r="C117" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D117" s="3">
         <v>1</v>
@@ -9085,7 +9085,7 @@
         <v>253</v>
       </c>
       <c r="C118" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D118" s="3">
         <v>1</v>
@@ -9150,7 +9150,7 @@
         <v>255</v>
       </c>
       <c r="C119" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D119" s="3">
         <v>1</v>
@@ -9540,7 +9540,7 @@
         <v>267</v>
       </c>
       <c r="C125" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D125" s="3">
         <v>-1</v>

</xml_diff>